<commit_message>
ASP.NET Core Fundamentals - CH4
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E60B2C7-B223-43BC-AF22-512555E96AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02FE01A2-8048-4091-89E8-9045BA550196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,14 @@
     <t>To do</t>
   </si>
   <si>
-    <t>Chapter 4 - start</t>
+    <t>Chapter 4 - Following the POST-GET-REDIRECT Pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -51,13 +51,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -69,13 +89,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -390,21 +413,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDFC62A-0F72-4B3A-9569-C3EE5DFE61E6}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -418,5 +439,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add WPF tutorial progress
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CBAC5B-2EDF-4B00-8843-4FED7A16286E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD38C0-5240-4379-828A-72EEB064FC45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
+    <workbookView xWindow="1308" yWindow="2796" windowWidth="21744" windowHeight="10176" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Course</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Ch 5 - START</t>
+  </si>
+  <si>
+    <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
+  </si>
+  <si>
+    <t>CH 4 - START</t>
   </si>
 </sst>
 </file>
@@ -411,15 +417,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CDFC62A-0F72-4B3A-9569-C3EE5DFE61E6}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -439,6 +445,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
WPF - end CH4
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BD38C0-5240-4379-828A-72EEB064FC45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02DE1A-5FC4-4229-AA3B-15A7FB2184E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1308" yWindow="2796" windowWidth="21744" windowHeight="10176" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Course</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
-  </si>
-  <si>
-    <t>CH 4 - START</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WPF Ch 5 complete
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC02DE1A-5FC4-4229-AA3B-15A7FB2184E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7422C62-A640-4353-848F-671B56235F21}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Course</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
+  </si>
+  <si>
+    <t>Ch 6 - START</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WPF Ch 8 done
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6440CFFF-0AA5-4D9D-BE78-548307A3CD4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A1FE97-3598-4866-9DAF-EF11A8860807}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
   </si>
   <si>
-    <t>Ch 8 - START</t>
+    <t>Ch 9 - START</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
WPF Ch 10 done
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A1FE97-3598-4866-9DAF-EF11A8860807}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFAE69C-F855-4727-973B-4635EE9AE510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
   </si>
   <si>
-    <t>Ch 9 - START</t>
+    <t>Ch 11 - START</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
WPF Ch 11 done
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFAE69C-F855-4727-973B-4635EE9AE510}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65610E05-9041-41C3-9D95-5C6FA198FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
+    <workbookView xWindow="6540" yWindow="4476" windowWidth="23040" windowHeight="12204" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
   </si>
   <si>
-    <t>Ch 11 - START</t>
+    <t>Ch 12 - START</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
WPF Ch 12 done
</commit_message>
<xml_diff>
--- a/Pluralsight Progress.xlsx
+++ b/Pluralsight Progress.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Study\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65610E05-9041-41C3-9D95-5C6FA198FCFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4AD3A1-2251-47DD-A658-021F499CE46C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6540" yWindow="4476" windowWidth="23040" windowHeight="12204" xr2:uid="{6BA806D8-2B4F-4058-B178-2AF5BC82B943}"/>
   </bookViews>
@@ -42,7 +42,7 @@
     <t>Building an Enterprise App with WPF, MVVM, and Entity Framework Code First</t>
   </si>
   <si>
-    <t>Ch 12 - START</t>
+    <t>Ch 13 - START</t>
   </si>
 </sst>
 </file>

</xml_diff>